<commit_message>
Add new grants taxonomy from nancy.  Todo is feedback from the CMs
</commit_message>
<xml_diff>
--- a/static/GT180116.xlsx
+++ b/static/GT180116.xlsx
@@ -24622,8 +24622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H8" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="N8" sqref="A8:N11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>